<commit_message>
fix excel input of variables + make diagramm (tablitsa)0.1.8.0
</commit_message>
<xml_diff>
--- a/ОценочныеКритерииПрочностиПути.XLSX
+++ b/ОценочныеКритерииПрочностиПути.XLSX
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Локомотив" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="10">
   <si>
     <t>Критерии</t>
   </si>
@@ -42,6 +42,9 @@
   </si>
   <si>
     <t>[бh]</t>
+  </si>
+  <si>
+    <t>[бз]</t>
   </si>
 </sst>
 </file>
@@ -49,7 +52,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="170" formatCode="0.0"/>
+    <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -83,7 +86,7 @@
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -390,8 +393,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -491,8 +494,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -567,7 +570,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B5">
         <v>0.8</v>

</xml_diff>